<commit_message>
fix port declare issues
</commit_message>
<xml_diff>
--- a/test/test.xlsx
+++ b/test/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\00DATA\00Project\xlsx2rtl\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22DC9A8C-31E8-47E1-BB19-0E1000064E7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18566F0C-2886-4065-809B-25B6955DE1B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -636,7 +636,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
add feature: truncate "reserved" fields, re-organize code structure
</commit_message>
<xml_diff>
--- a/test/test.xlsx
+++ b/test/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\00DATA\00Project\xlsx2rtl\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F027FB8-6FE9-4536-9B8D-C8A5C7B756E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C521BCC-E44C-4811-BEE0-01557D70F88B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="44">
   <si>
     <t>Description</t>
   </si>
@@ -126,21 +126,12 @@
     <t>portA[ 3: 0]</t>
   </si>
   <si>
-    <t>portB[ 4: 0]</t>
-  </si>
-  <si>
-    <t>portB[ 6: 5]</t>
-  </si>
-  <si>
     <t>portA[ 7: 4]</t>
   </si>
   <si>
     <t>reserved</t>
   </si>
   <si>
-    <t>portB[7   ]</t>
-  </si>
-  <si>
     <t>portC[5: 0]</t>
   </si>
   <si>
@@ -148,6 +139,24 @@
   </si>
   <si>
     <t>0x4</t>
+  </si>
+  <si>
+    <t>REG3</t>
+  </si>
+  <si>
+    <t>0x8</t>
+  </si>
+  <si>
+    <t>[ 31: 0]</t>
+  </si>
+  <si>
+    <t>portD[31:0]</t>
+  </si>
+  <si>
+    <t>portB[ 1: 0]</t>
+  </si>
+  <si>
+    <t>portB[2   ]</t>
   </si>
 </sst>
 </file>
@@ -539,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -639,7 +648,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>27</v>
@@ -650,9 +659,7 @@
       <c r="E5" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="9" t="s">
-        <v>33</v>
-      </c>
+      <c r="F5" s="9"/>
       <c r="G5" s="11" t="s">
         <v>5</v>
       </c>
@@ -671,10 +678,10 @@
         <v>3</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="G6" s="11" t="s">
         <v>5</v>
@@ -685,7 +692,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>24</v>
@@ -720,7 +727,7 @@
         <v>23</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
@@ -746,7 +753,7 @@
         <v>4</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G10" s="11" t="s">
         <v>5</v>
@@ -769,7 +776,7 @@
         <v>22</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="G11" s="11" t="s">
         <v>5</v>
@@ -792,7 +799,7 @@
         <v>4</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G12" s="11" t="s">
         <v>5</v>
@@ -815,7 +822,7 @@
         <v>4</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G13" s="11" t="s">
         <v>5</v>
@@ -832,6 +839,57 @@
       <c r="F14" s="9"/>
       <c r="G14" s="11"/>
     </row>
+    <row r="15" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+      <c r="A16" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="11"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>